<commit_message>
erd and changes in gantt_chart
</commit_message>
<xml_diff>
--- a/Documents/SE Project Gantt Chart Final.xlsx
+++ b/Documents/SE Project Gantt Chart Final.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7604492F-36FB-4DB1-93C1-26A399D24CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5D3CBF-32E9-49F0-945A-BACADBED85A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>PROJECT: HealthFlow Connect</t>
   </si>
@@ -230,10 +228,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="d"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,7 +516,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -597,7 +595,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -642,7 +640,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2157,28 +2155,28 @@
   </sheetPr>
   <dimension ref="A1:CM40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B22" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" style="2" customWidth="1"/>
-    <col min="10" max="64" width="3.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" style="2" customWidth="1"/>
+    <col min="10" max="64" width="3.5546875" style="2" customWidth="1"/>
     <col min="65" max="81" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="82" max="91" width="3.5703125" style="2" customWidth="1"/>
-    <col min="92" max="16384" width="8.85546875" style="2"/>
+    <col min="82" max="91" width="3.5546875" style="2" customWidth="1"/>
+    <col min="92" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:91" ht="25.15" customHeight="1"/>
-    <row r="2" spans="1:91" ht="49.9" customHeight="1">
+    <row r="1" spans="1:91" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:91" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="45" t="s">
         <v>0</v>
@@ -2203,7 +2201,7 @@
       <c r="T2" s="47"/>
       <c r="U2" s="47"/>
     </row>
-    <row r="3" spans="1:91" ht="19.899999999999999" customHeight="1">
+    <row r="3" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -2218,7 +2216,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:91" ht="30" customHeight="1">
+    <row r="4" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="11" t="s">
         <v>1</v>
@@ -2260,7 +2258,7 @@
       <c r="AF4" s="44"/>
       <c r="AG4" s="44"/>
     </row>
-    <row r="5" spans="1:91" ht="30" customHeight="1">
+    <row r="5" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="15" t="s">
         <v>8</v>
@@ -2279,7 +2277,7 @@
       <c r="CL5" s="39"/>
       <c r="CM5" s="39"/>
     </row>
-    <row r="6" spans="1:91" ht="30" customHeight="1">
+    <row r="6" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="16" t="s">
         <v>9</v>
@@ -2398,7 +2396,7 @@
       <c r="CL6" s="42"/>
       <c r="CM6" s="43"/>
     </row>
-    <row r="7" spans="1:91" ht="30" customHeight="1">
+    <row r="7" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="16" t="s">
         <v>11</v>
@@ -2738,7 +2736,7 @@
         <v>45392</v>
       </c>
     </row>
-    <row r="8" spans="1:91" ht="19.899999999999999" customHeight="1">
+    <row r="8" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -2828,7 +2826,7 @@
       <c r="CL8" s="23"/>
       <c r="CM8" s="23"/>
     </row>
-    <row r="9" spans="1:91" ht="40.15" customHeight="1">
+    <row r="9" spans="1:91" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="24" t="s">
         <v>12</v>
@@ -3181,7 +3179,7 @@
         <v>W</v>
       </c>
     </row>
-    <row r="10" spans="1:91" ht="30" hidden="1" customHeight="1">
+    <row r="10" spans="1:91" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="31"/>
@@ -3272,7 +3270,7 @@
       <c r="CL10" s="9"/>
       <c r="CM10" s="9"/>
     </row>
-    <row r="11" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="11" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="34" t="s">
         <v>19</v>
@@ -3613,7 +3611,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="12" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="36" t="s">
         <v>20</v>
@@ -3967,7 +3965,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="13" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="36" t="s">
         <v>23</v>
@@ -4320,7 +4318,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="14" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="36" t="s">
         <v>26</v>
@@ -4673,7 +4671,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="15" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="36" t="s">
         <v>29</v>
@@ -5026,7 +5024,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="16" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="36" t="s">
         <v>31</v>
@@ -5379,7 +5377,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="17" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="36" t="s">
         <v>32</v>
@@ -5484,7 +5482,7 @@
       <c r="CL17" s="6"/>
       <c r="CM17" s="6"/>
     </row>
-    <row r="18" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="18" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="34" t="s">
         <v>33</v>
@@ -5825,7 +5823,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="19" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="36" t="s">
         <v>34</v>
@@ -6178,7 +6176,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="20" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="36" t="s">
         <v>35</v>
@@ -6531,7 +6529,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="21" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="36" t="s">
         <v>37</v>
@@ -6546,7 +6544,7 @@
         <v>38</v>
       </c>
       <c r="F21" s="37">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G21" s="32">
         <v>45325</v>
@@ -6884,7 +6882,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="22" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="36" t="s">
         <v>39</v>
@@ -6899,7 +6897,7 @@
         <v>40</v>
       </c>
       <c r="F22" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="32">
         <v>45327</v>
@@ -7237,7 +7235,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="23" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="36" t="s">
         <v>41</v>
@@ -7245,10 +7243,14 @@
       <c r="C23" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="D23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="F23" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="32">
         <v>45332</v>
@@ -7586,7 +7588,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="24" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="36" t="s">
         <v>43</v>
@@ -7594,10 +7596,14 @@
       <c r="C24" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
+      <c r="D24" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>30</v>
+      </c>
       <c r="F24" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="32">
         <v>45332</v>
@@ -7689,7 +7695,7 @@
       <c r="CL24" s="6"/>
       <c r="CM24" s="6"/>
     </row>
-    <row r="25" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="25" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="36" t="s">
         <v>44</v>
@@ -7792,7 +7798,7 @@
       <c r="CL25" s="6"/>
       <c r="CM25" s="6"/>
     </row>
-    <row r="26" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="26" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="34" t="s">
         <v>45</v>
@@ -8133,7 +8139,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="27" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="36" t="s">
         <v>46</v>
@@ -8482,7 +8488,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="28" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="36" t="s">
         <v>47</v>
@@ -8831,7 +8837,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="29" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="36" t="s">
         <v>48</v>
@@ -9180,7 +9186,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="30" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="34" t="s">
         <v>49</v>
@@ -9521,7 +9527,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="31" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="36" t="s">
         <v>50</v>
@@ -9870,7 +9876,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="32" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="36" t="s">
         <v>51</v>
@@ -10219,7 +10225,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="33" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="36" t="s">
         <v>52</v>
@@ -10568,7 +10574,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="34" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="36" t="s">
         <v>53</v>
@@ -10917,7 +10923,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="35" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="36" t="s">
         <v>54</v>
@@ -11266,7 +11272,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="36" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="34" t="s">
         <v>56</v>
@@ -11607,7 +11613,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="37" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="38" t="s">
         <v>57</v>
@@ -11710,7 +11716,7 @@
       <c r="CL37" s="6"/>
       <c r="CM37" s="6"/>
     </row>
-    <row r="38" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="38" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="38" t="s">
         <v>58</v>
@@ -11813,7 +11819,7 @@
       <c r="CL38" s="6"/>
       <c r="CM38" s="6"/>
     </row>
-    <row r="39" spans="1:91" s="9" customFormat="1" ht="40.15" customHeight="1">
+    <row r="39" spans="1:91" s="9" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="38" t="s">
         <v>60</v>
@@ -12162,7 +12168,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:91" ht="30" customHeight="1">
+    <row r="40" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D40" s="28"/>
       <c r="E40" s="28"/>
     </row>
@@ -12512,35 +12518,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -12840,16 +12817,74 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF181E67-B5A5-4E32-9D0A-4494603D7B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF181E67-B5A5-4E32-9D0A-4494603D7B36}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>